<commit_message>
Futher harmonizing MC dataset with collector
</commit_message>
<xml_diff>
--- a/inst/survey/survey.xlsx
+++ b/inst/survey/survey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dseversk/rstats/evaluator/inst/survey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C2C289-9D62-C447-91BE-B8D6E89910ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8439BD69-7ABE-B540-A652-162AB5D17E4B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40240" yWindow="-1020" windowWidth="21760" windowHeight="17900" firstSheet="4" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40240" yWindow="-1020" windowWidth="21760" windowHeight="17900" firstSheet="4" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="18" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="275">
   <si>
     <t>Threats</t>
   </si>
@@ -133,9 +133,6 @@
     <t>Inadequate response results in inappropriate internal use of data.</t>
   </si>
   <si>
-    <t>External Legal Authority</t>
-  </si>
-  <si>
     <t>Inability to respond to litgation holds.</t>
   </si>
   <si>
@@ -704,6 +701,177 @@
   </si>
   <si>
     <t>Environmental</t>
+  </si>
+  <si>
+    <t>External Litigants</t>
+  </si>
+  <si>
+    <t>RS-54</t>
+  </si>
+  <si>
+    <t>RS-48</t>
+  </si>
+  <si>
+    <t>RS-51</t>
+  </si>
+  <si>
+    <t>RS-24</t>
+  </si>
+  <si>
+    <t>RS-25</t>
+  </si>
+  <si>
+    <t>RS-26</t>
+  </si>
+  <si>
+    <t>RS-27</t>
+  </si>
+  <si>
+    <t>RS-13</t>
+  </si>
+  <si>
+    <t>RS-14</t>
+  </si>
+  <si>
+    <t>RS-15</t>
+  </si>
+  <si>
+    <t>RS-16</t>
+  </si>
+  <si>
+    <t>RS-6</t>
+  </si>
+  <si>
+    <t>RS-7</t>
+  </si>
+  <si>
+    <t>RS-8</t>
+  </si>
+  <si>
+    <t>RS-01</t>
+  </si>
+  <si>
+    <t>RS-02</t>
+  </si>
+  <si>
+    <t>RS-03</t>
+  </si>
+  <si>
+    <t>RS-04</t>
+  </si>
+  <si>
+    <t>RS-05</t>
+  </si>
+  <si>
+    <t>RS-09</t>
+  </si>
+  <si>
+    <t>RS-10</t>
+  </si>
+  <si>
+    <t>RS-11</t>
+  </si>
+  <si>
+    <t>RS-12</t>
+  </si>
+  <si>
+    <t>RS-45</t>
+  </si>
+  <si>
+    <t>RS-46</t>
+  </si>
+  <si>
+    <t>RS-47</t>
+  </si>
+  <si>
+    <t>RS-41</t>
+  </si>
+  <si>
+    <t>RS-42</t>
+  </si>
+  <si>
+    <t>RS-43</t>
+  </si>
+  <si>
+    <t>RS-44</t>
+  </si>
+  <si>
+    <t>RS-32</t>
+  </si>
+  <si>
+    <t>RS-33</t>
+  </si>
+  <si>
+    <t>RS-34</t>
+  </si>
+  <si>
+    <t>RS-35</t>
+  </si>
+  <si>
+    <t>RS-36</t>
+  </si>
+  <si>
+    <t>RS-28</t>
+  </si>
+  <si>
+    <t>RS-29</t>
+  </si>
+  <si>
+    <t>RS-30</t>
+  </si>
+  <si>
+    <t>RS-56</t>
+  </si>
+  <si>
+    <t>RS-19</t>
+  </si>
+  <si>
+    <t>RS-20</t>
+  </si>
+  <si>
+    <t>RS-21</t>
+  </si>
+  <si>
+    <t>RS-22</t>
+  </si>
+  <si>
+    <t>RS-23</t>
+  </si>
+  <si>
+    <t>RS-50</t>
+  </si>
+  <si>
+    <t>RS-52</t>
+  </si>
+  <si>
+    <t>RS-53</t>
+  </si>
+  <si>
+    <t>RS-37</t>
+  </si>
+  <si>
+    <t>RS-38</t>
+  </si>
+  <si>
+    <t>RS-39</t>
+  </si>
+  <si>
+    <t>RS-40</t>
+  </si>
+  <si>
+    <t>RS-55</t>
+  </si>
+  <si>
+    <t>RS-31</t>
+  </si>
+  <si>
+    <t>RS-17</t>
+  </si>
+  <si>
+    <t>RS-18</t>
+  </si>
+  <si>
+    <t>RS-49</t>
   </si>
 </sst>
 </file>
@@ -2106,144 +2274,144 @@
   <sheetData>
     <row r="1" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>124</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -2281,7 +2449,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2296,7 +2464,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -2313,18 +2481,18 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3">
         <v>8</v>
@@ -2332,13 +2500,13 @@
     </row>
     <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>13</v>
@@ -2375,15 +2543,15 @@
         <v>15</v>
       </c>
       <c r="G7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -2394,11 +2562,11 @@
       <c r="E8" t="s">
         <v>11</v>
       </c>
-      <c r="F8">
-        <v>9</v>
+      <c r="F8" t="s">
+        <v>238</v>
       </c>
       <c r="G8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -2406,7 +2574,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -2417,11 +2585,11 @@
       <c r="E9" t="s">
         <v>9</v>
       </c>
-      <c r="F9">
-        <v>10</v>
+      <c r="F9" t="s">
+        <v>239</v>
       </c>
       <c r="G9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -2429,7 +2597,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -2440,11 +2608,11 @@
       <c r="E10" t="s">
         <v>9</v>
       </c>
-      <c r="F10">
-        <v>11</v>
+      <c r="F10" t="s">
+        <v>240</v>
       </c>
       <c r="G10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -2452,7 +2620,7 @@
         <v>17</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -2463,11 +2631,11 @@
       <c r="E11" t="s">
         <v>9</v>
       </c>
-      <c r="F11">
-        <v>12</v>
+      <c r="F11" t="s">
+        <v>241</v>
       </c>
       <c r="G11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2503,7 +2671,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2518,7 +2686,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -2535,18 +2703,18 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3">
         <v>56</v>
@@ -2554,13 +2722,13 @@
     </row>
     <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>39</v>
@@ -2600,15 +2768,15 @@
         <v>15</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -2619,19 +2787,19 @@
       <c r="E8" t="s">
         <v>10</v>
       </c>
-      <c r="F8">
-        <v>45</v>
+      <c r="F8" t="s">
+        <v>242</v>
       </c>
       <c r="G8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -2642,19 +2810,19 @@
       <c r="E9" t="s">
         <v>10</v>
       </c>
-      <c r="F9">
-        <v>46</v>
+      <c r="F9" t="s">
+        <v>243</v>
       </c>
       <c r="G9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -2665,11 +2833,11 @@
       <c r="E10" t="s">
         <v>9</v>
       </c>
-      <c r="F10">
-        <v>47</v>
+      <c r="F10" t="s">
+        <v>244</v>
       </c>
       <c r="G10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -2705,7 +2873,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2720,7 +2888,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="20" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -2737,18 +2905,18 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3">
         <v>52</v>
@@ -2756,13 +2924,13 @@
     </row>
     <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>53</v>
@@ -2770,13 +2938,13 @@
     </row>
     <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5">
         <v>54</v>
@@ -2784,13 +2952,13 @@
     </row>
     <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6">
         <v>55</v>
@@ -2827,15 +2995,15 @@
         <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -2846,19 +3014,19 @@
       <c r="E10" t="s">
         <v>9</v>
       </c>
-      <c r="F10">
-        <v>41</v>
+      <c r="F10" t="s">
+        <v>245</v>
       </c>
       <c r="G10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -2869,19 +3037,19 @@
       <c r="E11" t="s">
         <v>11</v>
       </c>
-      <c r="F11">
-        <v>42</v>
+      <c r="F11" t="s">
+        <v>246</v>
       </c>
       <c r="G11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -2892,19 +3060,19 @@
       <c r="E12" t="s">
         <v>9</v>
       </c>
-      <c r="F12">
-        <v>43</v>
+      <c r="F12" t="s">
+        <v>247</v>
       </c>
       <c r="G12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -2915,11 +3083,11 @@
       <c r="E13" t="s">
         <v>9</v>
       </c>
-      <c r="F13">
-        <v>44</v>
+      <c r="F13" t="s">
+        <v>248</v>
       </c>
       <c r="G13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2955,7 +3123,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2970,7 +3138,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="20" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -2987,18 +3155,18 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3">
         <v>37</v>
@@ -3006,13 +3174,13 @@
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>40</v>
@@ -3020,13 +3188,13 @@
     </row>
     <row r="5" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5">
         <v>42</v>
@@ -3034,13 +3202,13 @@
     </row>
     <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6">
         <v>43</v>
@@ -3048,13 +3216,13 @@
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7">
         <v>46</v>
@@ -3062,13 +3230,13 @@
     </row>
     <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8">
         <v>47</v>
@@ -3076,13 +3244,13 @@
     </row>
     <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9">
         <v>48</v>
@@ -3090,13 +3258,13 @@
     </row>
     <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10">
         <v>49</v>
@@ -3104,13 +3272,13 @@
     </row>
     <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11">
         <v>50</v>
@@ -3118,13 +3286,13 @@
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12">
         <v>51</v>
@@ -3132,13 +3300,13 @@
     </row>
     <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13">
         <v>33</v>
@@ -3146,13 +3314,13 @@
     </row>
     <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14">
         <v>34</v>
@@ -3160,13 +3328,13 @@
     </row>
     <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15">
         <v>35</v>
@@ -3174,13 +3342,13 @@
     </row>
     <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16">
         <v>36</v>
@@ -3220,15 +3388,15 @@
         <v>15</v>
       </c>
       <c r="G19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
@@ -3239,19 +3407,19 @@
       <c r="E20" t="s">
         <v>9</v>
       </c>
-      <c r="F20">
-        <v>32</v>
+      <c r="F20" t="s">
+        <v>249</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
@@ -3262,19 +3430,19 @@
       <c r="E21" t="s">
         <v>10</v>
       </c>
-      <c r="F21">
-        <v>33</v>
+      <c r="F21" t="s">
+        <v>250</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
@@ -3285,19 +3453,19 @@
       <c r="E22" t="s">
         <v>9</v>
       </c>
-      <c r="F22">
-        <v>34</v>
+      <c r="F22" t="s">
+        <v>251</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
@@ -3308,19 +3476,19 @@
       <c r="E23" t="s">
         <v>10</v>
       </c>
-      <c r="F23">
-        <v>35</v>
+      <c r="F23" t="s">
+        <v>252</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
@@ -3331,19 +3499,19 @@
       <c r="E24" t="s">
         <v>10</v>
       </c>
-      <c r="F24">
-        <v>36</v>
+      <c r="F24" t="s">
+        <v>253</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C25" t="s">
         <v>7</v>
@@ -3354,19 +3522,19 @@
       <c r="E25" t="s">
         <v>10</v>
       </c>
-      <c r="F25">
-        <v>28</v>
+      <c r="F25" t="s">
+        <v>254</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B26" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C26" t="s">
         <v>12</v>
@@ -3377,19 +3545,19 @@
       <c r="E26" t="s">
         <v>10</v>
       </c>
-      <c r="F26">
-        <v>29</v>
+      <c r="F26" t="s">
+        <v>255</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C27" t="s">
         <v>12</v>
@@ -3400,11 +3568,11 @@
       <c r="E27" t="s">
         <v>9</v>
       </c>
-      <c r="F27">
-        <v>30</v>
+      <c r="F27" t="s">
+        <v>256</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -3439,7 +3607,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3453,7 +3621,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="20" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -3470,18 +3638,18 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3">
         <v>38</v>
@@ -3489,13 +3657,13 @@
     </row>
     <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>44</v>
@@ -3532,15 +3700,15 @@
         <v>15</v>
       </c>
       <c r="G7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -3551,11 +3719,11 @@
       <c r="E8" t="s">
         <v>9</v>
       </c>
-      <c r="F8">
-        <v>56</v>
+      <c r="F8" t="s">
+        <v>257</v>
       </c>
       <c r="G8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -3590,8 +3758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3606,7 +3774,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -3623,18 +3791,18 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3">
         <v>25</v>
@@ -3642,13 +3810,13 @@
     </row>
     <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>26</v>
@@ -3656,13 +3824,13 @@
     </row>
     <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5">
         <v>27</v>
@@ -3670,13 +3838,13 @@
     </row>
     <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6">
         <v>28</v>
@@ -3684,13 +3852,13 @@
     </row>
     <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7">
         <v>59</v>
@@ -3727,15 +3895,15 @@
         <v>15</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -3746,19 +3914,19 @@
       <c r="E11" t="s">
         <v>10</v>
       </c>
-      <c r="F11">
-        <v>19</v>
+      <c r="F11" t="s">
+        <v>258</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -3769,11 +3937,11 @@
       <c r="E12" t="s">
         <v>9</v>
       </c>
-      <c r="F12">
-        <v>20</v>
+      <c r="F12" t="s">
+        <v>259</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -3781,7 +3949,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -3792,19 +3960,19 @@
       <c r="E13" t="s">
         <v>9</v>
       </c>
-      <c r="F13">
-        <v>21</v>
+      <c r="F13" t="s">
+        <v>260</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
@@ -3815,11 +3983,11 @@
       <c r="E14" t="s">
         <v>9</v>
       </c>
-      <c r="F14">
-        <v>22</v>
+      <c r="F14" t="s">
+        <v>261</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -3827,7 +3995,7 @@
         <v>26</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
@@ -3838,11 +4006,11 @@
       <c r="E15" t="s">
         <v>9</v>
       </c>
-      <c r="F15">
-        <v>23</v>
+      <c r="F15" t="s">
+        <v>262</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -3850,7 +4018,7 @@
         <v>27</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
@@ -3861,19 +4029,19 @@
       <c r="E16" t="s">
         <v>9</v>
       </c>
-      <c r="F16">
-        <v>50</v>
+      <c r="F16" t="s">
+        <v>263</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>28</v>
+        <v>218</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -3884,8 +4052,8 @@
       <c r="E17" t="s">
         <v>9</v>
       </c>
-      <c r="F17">
-        <v>52</v>
+      <c r="F17" t="s">
+        <v>264</v>
       </c>
       <c r="G17" s="3">
         <v>59</v>
@@ -3893,10 +4061,10 @@
     </row>
     <row r="18" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
@@ -3907,8 +4075,8 @@
       <c r="E18" t="s">
         <v>10</v>
       </c>
-      <c r="F18">
-        <v>53</v>
+      <c r="F18" t="s">
+        <v>265</v>
       </c>
       <c r="G18" s="3">
         <v>59</v>
@@ -3916,10 +4084,10 @@
     </row>
     <row r="19" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
@@ -3930,19 +4098,19 @@
       <c r="E19" t="s">
         <v>9</v>
       </c>
-      <c r="F19">
-        <v>37</v>
+      <c r="F19" t="s">
+        <v>266</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
@@ -3953,19 +4121,19 @@
       <c r="E20" t="s">
         <v>9</v>
       </c>
-      <c r="F20">
-        <v>38</v>
+      <c r="F20" t="s">
+        <v>267</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
@@ -3976,19 +4144,19 @@
       <c r="E21" t="s">
         <v>10</v>
       </c>
-      <c r="F21">
-        <v>39</v>
+      <c r="F21" t="s">
+        <v>268</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
@@ -3999,11 +4167,11 @@
       <c r="E22" t="s">
         <v>9</v>
       </c>
-      <c r="F22">
-        <v>40</v>
+      <c r="F22" t="s">
+        <v>269</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -4039,7 +4207,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4053,7 +4221,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="20" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -4070,18 +4238,18 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3">
         <v>41</v>
@@ -4089,13 +4257,13 @@
     </row>
     <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>45</v>
@@ -4132,15 +4300,15 @@
         <v>15</v>
       </c>
       <c r="G7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -4151,19 +4319,19 @@
       <c r="E8" t="s">
         <v>11</v>
       </c>
-      <c r="F8">
-        <v>55</v>
+      <c r="F8" t="s">
+        <v>270</v>
       </c>
       <c r="G8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -4174,11 +4342,11 @@
       <c r="E9" t="s">
         <v>9</v>
       </c>
-      <c r="F9">
-        <v>31</v>
+      <c r="F9" t="s">
+        <v>271</v>
       </c>
       <c r="G9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -4213,8 +4381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4229,7 +4397,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -4246,18 +4414,18 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3">
         <v>21</v>
@@ -4265,13 +4433,13 @@
     </row>
     <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>22</v>
@@ -4279,13 +4447,13 @@
     </row>
     <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5">
         <v>23</v>
@@ -4293,13 +4461,13 @@
     </row>
     <row r="6" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6">
         <v>24</v>
@@ -4336,7 +4504,7 @@
         <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -4344,7 +4512,7 @@
         <v>22</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -4355,11 +4523,11 @@
       <c r="E10" t="s">
         <v>9</v>
       </c>
-      <c r="F10">
-        <v>17</v>
+      <c r="F10" t="s">
+        <v>272</v>
       </c>
       <c r="G10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -4367,7 +4535,7 @@
         <v>23</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -4378,11 +4546,11 @@
       <c r="E11" t="s">
         <v>9</v>
       </c>
-      <c r="F11">
-        <v>18</v>
+      <c r="F11" t="s">
+        <v>273</v>
       </c>
       <c r="G11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -4390,7 +4558,7 @@
         <v>24</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
@@ -4401,11 +4569,11 @@
       <c r="E12" t="s">
         <v>9</v>
       </c>
-      <c r="F12">
-        <v>49</v>
+      <c r="F12" t="s">
+        <v>274</v>
       </c>
       <c r="G12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -4452,59 +4620,59 @@
   <sheetData>
     <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B1" s="10"/>
     </row>
     <row r="3" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B3" s="11"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B10" s="11"/>
     </row>
@@ -4513,7 +4681,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -4521,7 +4689,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -4529,12 +4697,12 @@
         <v>10</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B15" s="11"/>
     </row>
@@ -4543,7 +4711,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -4551,7 +4719,7 @@
         <v>12</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -4559,12 +4727,12 @@
         <v>8</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B20" s="11"/>
     </row>
@@ -4573,7 +4741,7 @@
         <v>11</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -4581,7 +4749,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -4589,7 +4757,7 @@
         <v>10</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -4691,27 +4859,27 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -4724,7 +4892,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4739,7 +4907,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -4756,18 +4924,18 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -4775,13 +4943,13 @@
     </row>
     <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>4</v>
@@ -4789,13 +4957,13 @@
     </row>
     <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5">
         <v>6</v>
@@ -4832,15 +5000,15 @@
         <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -4851,11 +5019,11 @@
       <c r="E9" t="s">
         <v>9</v>
       </c>
-      <c r="F9">
-        <v>54</v>
+      <c r="F9" t="s">
+        <v>219</v>
       </c>
       <c r="G9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -4891,7 +5059,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4906,7 +5074,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -4923,18 +5091,18 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3">
         <v>57</v>
@@ -4942,13 +5110,13 @@
     </row>
     <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>58</v>
@@ -4985,15 +5153,15 @@
         <v>15</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -5004,19 +5172,19 @@
       <c r="E8" t="s">
         <v>9</v>
       </c>
-      <c r="F8">
-        <v>48</v>
+      <c r="F8" t="s">
+        <v>220</v>
       </c>
       <c r="G8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -5027,11 +5195,11 @@
       <c r="E9" t="s">
         <v>9</v>
       </c>
-      <c r="F9">
-        <v>51</v>
+      <c r="F9" t="s">
+        <v>221</v>
       </c>
       <c r="G9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -5067,7 +5235,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5082,7 +5250,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -5099,18 +5267,18 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3">
         <v>29</v>
@@ -5118,13 +5286,13 @@
     </row>
     <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>30</v>
@@ -5132,13 +5300,13 @@
     </row>
     <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5">
         <v>31</v>
@@ -5146,13 +5314,13 @@
     </row>
     <row r="6" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6">
         <v>60</v>
@@ -5189,15 +5357,15 @@
         <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
@@ -5208,19 +5376,19 @@
       <c r="E10" t="s">
         <v>10</v>
       </c>
-      <c r="F10">
-        <v>24</v>
+      <c r="F10" t="s">
+        <v>222</v>
       </c>
       <c r="G10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -5231,19 +5399,19 @@
       <c r="E11" t="s">
         <v>9</v>
       </c>
-      <c r="F11">
-        <v>25</v>
+      <c r="F11" t="s">
+        <v>223</v>
       </c>
       <c r="G11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -5254,19 +5422,19 @@
       <c r="E12" t="s">
         <v>9</v>
       </c>
-      <c r="F12">
-        <v>26</v>
+      <c r="F12" t="s">
+        <v>224</v>
       </c>
       <c r="G12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -5277,11 +5445,11 @@
       <c r="E13" t="s">
         <v>10</v>
       </c>
-      <c r="F13">
-        <v>27</v>
+      <c r="F13" t="s">
+        <v>225</v>
       </c>
       <c r="G13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -5317,7 +5485,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5333,7 +5501,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -5350,18 +5518,18 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3">
         <v>17</v>
@@ -5369,13 +5537,13 @@
     </row>
     <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>18</v>
@@ -5383,13 +5551,13 @@
     </row>
     <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5">
         <v>19</v>
@@ -5397,13 +5565,13 @@
     </row>
     <row r="6" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6">
         <v>20</v>
@@ -5440,15 +5608,15 @@
         <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -5459,11 +5627,11 @@
       <c r="E10" t="s">
         <v>10</v>
       </c>
-      <c r="F10">
-        <v>13</v>
+      <c r="F10" t="s">
+        <v>226</v>
       </c>
       <c r="G10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -5471,7 +5639,7 @@
         <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -5482,11 +5650,11 @@
       <c r="E11" t="s">
         <v>9</v>
       </c>
-      <c r="F11">
-        <v>14</v>
+      <c r="F11" t="s">
+        <v>227</v>
       </c>
       <c r="G11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -5494,7 +5662,7 @@
         <v>20</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -5505,19 +5673,19 @@
       <c r="E12" t="s">
         <v>9</v>
       </c>
-      <c r="F12">
-        <v>15</v>
+      <c r="F12" t="s">
+        <v>228</v>
       </c>
       <c r="G12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -5528,11 +5696,11 @@
       <c r="E13" t="s">
         <v>9</v>
       </c>
-      <c r="F13">
-        <v>16</v>
+      <c r="F13" t="s">
+        <v>229</v>
       </c>
       <c r="G13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -5568,7 +5736,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5584,7 +5752,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -5601,18 +5769,18 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3">
         <v>9</v>
@@ -5620,13 +5788,13 @@
     </row>
     <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -5634,13 +5802,13 @@
     </row>
     <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5">
         <v>11</v>
@@ -5648,13 +5816,13 @@
     </row>
     <row r="6" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6">
         <v>12</v>
@@ -5694,15 +5862,15 @@
         <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -5713,19 +5881,19 @@
       <c r="E10" t="s">
         <v>10</v>
       </c>
-      <c r="F10">
-        <v>6</v>
+      <c r="F10" t="s">
+        <v>230</v>
       </c>
       <c r="G10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -5736,19 +5904,19 @@
       <c r="E11" t="s">
         <v>10</v>
       </c>
-      <c r="F11">
-        <v>7</v>
+      <c r="F11" t="s">
+        <v>231</v>
       </c>
       <c r="G11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
@@ -5759,11 +5927,11 @@
       <c r="E12" t="s">
         <v>10</v>
       </c>
-      <c r="F12">
-        <v>8</v>
+      <c r="F12" t="s">
+        <v>232</v>
       </c>
       <c r="G12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -5799,7 +5967,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5813,7 +5981,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="20" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -5830,18 +5998,18 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -5849,13 +6017,13 @@
     </row>
     <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -5863,13 +6031,13 @@
     </row>
     <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -5877,13 +6045,13 @@
     </row>
     <row r="6" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6">
         <v>7</v>
@@ -5891,13 +6059,13 @@
     </row>
     <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7">
         <v>32</v>
@@ -5905,13 +6073,13 @@
     </row>
     <row r="8" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8">
         <v>14</v>
@@ -5919,13 +6087,13 @@
     </row>
     <row r="9" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9">
         <v>15</v>
@@ -5933,13 +6101,13 @@
     </row>
     <row r="10" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10">
         <v>16</v>
@@ -5976,15 +6144,15 @@
         <v>15</v>
       </c>
       <c r="G13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
@@ -5995,19 +6163,19 @@
       <c r="E14" t="s">
         <v>9</v>
       </c>
-      <c r="F14">
-        <v>1</v>
+      <c r="F14" t="s">
+        <v>233</v>
       </c>
       <c r="G14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
@@ -6018,19 +6186,19 @@
       <c r="E15" t="s">
         <v>9</v>
       </c>
-      <c r="F15">
-        <v>2</v>
+      <c r="F15" t="s">
+        <v>234</v>
       </c>
       <c r="G15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
@@ -6041,11 +6209,11 @@
       <c r="E16" t="s">
         <v>9</v>
       </c>
-      <c r="F16">
-        <v>3</v>
+      <c r="F16" t="s">
+        <v>235</v>
       </c>
       <c r="G16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -6053,7 +6221,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
@@ -6064,19 +6232,19 @@
       <c r="E17" t="s">
         <v>9</v>
       </c>
-      <c r="F17">
-        <v>4</v>
+      <c r="F17" t="s">
+        <v>236</v>
       </c>
       <c r="G17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
@@ -6087,11 +6255,11 @@
       <c r="E18" t="s">
         <v>10</v>
       </c>
-      <c r="F18">
-        <v>5</v>
+      <c r="F18" t="s">
+        <v>237</v>
       </c>
       <c r="G18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Switch capability ids to use the CAP- prefix from collector
</commit_message>
<xml_diff>
--- a/inst/survey/survey.xlsx
+++ b/inst/survey/survey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dseversk/rstats/evaluator/inst/survey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8439BD69-7ABE-B540-A652-162AB5D17E4B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC4DCAD-26ED-B04E-905C-548B18E8C91E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40240" yWindow="-1020" windowWidth="21760" windowHeight="17900" firstSheet="4" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="18" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="335">
   <si>
     <t>Threats</t>
   </si>
@@ -187,18 +187,6 @@
     <t>CapabilityID</t>
   </si>
   <si>
-    <t>9, 10, 11, 12</t>
-  </si>
-  <si>
-    <t>17, 18, 19, 20</t>
-  </si>
-  <si>
-    <t>21, 22, 23, 24</t>
-  </si>
-  <si>
-    <t>57, 58</t>
-  </si>
-  <si>
     <t>Domain</t>
   </si>
   <si>
@@ -481,30 +469,6 @@
     <t>ORG</t>
   </si>
   <si>
-    <t>2, 4, 6</t>
-  </si>
-  <si>
-    <t>29, 30, 31, 60</t>
-  </si>
-  <si>
-    <t>8, 13</t>
-  </si>
-  <si>
-    <t>56, 39</t>
-  </si>
-  <si>
-    <t>52, 53, 54, 55</t>
-  </si>
-  <si>
-    <t>25, 26, 27, 28, 59</t>
-  </si>
-  <si>
-    <t>41, 45</t>
-  </si>
-  <si>
-    <t>37, 38, 40, 41, 42, 43, 46, 47, 48, 49, 50, 39, 51, 33, 34, 35, 36</t>
-  </si>
-  <si>
     <t>Unknown attack intelligence results in undetected events.</t>
   </si>
   <si>
@@ -532,9 +496,6 @@
     <t>Damage to or loss of information system due to natural disaster at physical facility.</t>
   </si>
   <si>
-    <t>38, 44</t>
-  </si>
-  <si>
     <t>Real and serious effect on the bottom line and/or long-term ability to generate revenue.</t>
   </si>
   <si>
@@ -625,33 +586,18 @@
     <t>Unauthorized access to or use of information and systems.</t>
   </si>
   <si>
-    <t>30, 31, 60</t>
-  </si>
-  <si>
     <t>Successful social engineering attacks result in information or financial loss.</t>
   </si>
   <si>
     <t>Security failure or instability of providers or partners results in disclosure of organizational data.</t>
   </si>
   <si>
-    <t>1, 7, 14, 15, 16</t>
-  </si>
-  <si>
-    <t>1, 3, 5, 7, 32, 14, 15, 16</t>
-  </si>
-  <si>
-    <t>1, 5, 7, 32, 14, 15, 16</t>
-  </si>
-  <si>
     <t>New or changing privacy regulations are not implemented in organizational IT systems.</t>
   </si>
   <si>
     <t>Lack of accountability for critical information and systems results in inappropriate control and inventory.</t>
   </si>
   <si>
-    <t>33, 34, 35, 36</t>
-  </si>
-  <si>
     <t>Undetected and unremediated security incidents result in unmitigated access.</t>
   </si>
   <si>
@@ -872,6 +818,240 @@
   </si>
   <si>
     <t>RS-49</t>
+  </si>
+  <si>
+    <t>CAP-2</t>
+  </si>
+  <si>
+    <t>CAP-4</t>
+  </si>
+  <si>
+    <t>CAP-6</t>
+  </si>
+  <si>
+    <t>CAP-2, CAP-4, CAP-6</t>
+  </si>
+  <si>
+    <t>CAP-57</t>
+  </si>
+  <si>
+    <t>CAP-58</t>
+  </si>
+  <si>
+    <t>CAP-57, CAP-58</t>
+  </si>
+  <si>
+    <t>CAP-29</t>
+  </si>
+  <si>
+    <t>CAP-30</t>
+  </si>
+  <si>
+    <t>CAP-31</t>
+  </si>
+  <si>
+    <t>CAP-60</t>
+  </si>
+  <si>
+    <t>CAP-30, CAP-31, CAP-60</t>
+  </si>
+  <si>
+    <t>CAP-29, CAP-30, CAP-31, CAP-60</t>
+  </si>
+  <si>
+    <t>CAP-17</t>
+  </si>
+  <si>
+    <t>CAP-18</t>
+  </si>
+  <si>
+    <t>CAP-19</t>
+  </si>
+  <si>
+    <t>CAP-20</t>
+  </si>
+  <si>
+    <t>CAP-17, CAP-18, CAP-19, CAP-20</t>
+  </si>
+  <si>
+    <t>CAP-09</t>
+  </si>
+  <si>
+    <t>CAP-10</t>
+  </si>
+  <si>
+    <t>CAP-11</t>
+  </si>
+  <si>
+    <t>CAP-12</t>
+  </si>
+  <si>
+    <t>CAP-09, CAP-10, CAP-11, CAP-12</t>
+  </si>
+  <si>
+    <t>CAP-01</t>
+  </si>
+  <si>
+    <t>CAP-03</t>
+  </si>
+  <si>
+    <t>CAP-05</t>
+  </si>
+  <si>
+    <t>CAP-07</t>
+  </si>
+  <si>
+    <t>CAP-32</t>
+  </si>
+  <si>
+    <t>CAP-14</t>
+  </si>
+  <si>
+    <t>CAP-15</t>
+  </si>
+  <si>
+    <t>CAP-16</t>
+  </si>
+  <si>
+    <t>CAP-01, CAP-05, CAP-07, CAP-32, CAP-14, CAP-15, CAP-16</t>
+  </si>
+  <si>
+    <t>CAP-01, CAP-07, CAP-14, CAP-15, CAP-16</t>
+  </si>
+  <si>
+    <t>CAP-08</t>
+  </si>
+  <si>
+    <t>CAP-13</t>
+  </si>
+  <si>
+    <t>CAP-56</t>
+  </si>
+  <si>
+    <t>CAP-39</t>
+  </si>
+  <si>
+    <t>CAP-56, CAP-39</t>
+  </si>
+  <si>
+    <t>CAP-52</t>
+  </si>
+  <si>
+    <t>CAP-53</t>
+  </si>
+  <si>
+    <t>CAP-54</t>
+  </si>
+  <si>
+    <t>CAP-55</t>
+  </si>
+  <si>
+    <t>CAP-52, CAP-53, CAP-54, CAP-55</t>
+  </si>
+  <si>
+    <t>CAP-37</t>
+  </si>
+  <si>
+    <t>CAP-40</t>
+  </si>
+  <si>
+    <t>CAP-42</t>
+  </si>
+  <si>
+    <t>CAP-43</t>
+  </si>
+  <si>
+    <t>CAP-46</t>
+  </si>
+  <si>
+    <t>CAP-47</t>
+  </si>
+  <si>
+    <t>CAP-48</t>
+  </si>
+  <si>
+    <t>CAP-49</t>
+  </si>
+  <si>
+    <t>CAP-50</t>
+  </si>
+  <si>
+    <t>CAP-51</t>
+  </si>
+  <si>
+    <t>CAP-33</t>
+  </si>
+  <si>
+    <t>CAP-34</t>
+  </si>
+  <si>
+    <t>CAP-35</t>
+  </si>
+  <si>
+    <t>CAP-36</t>
+  </si>
+  <si>
+    <t>CAP-37, CAP-38, CAP-40, CAP-41, CAP-42, CAP-43, CAP-46, CAP-47, CAP-48, CAP-49, CAP-50, CAP-39, CAP-51, CAP-33, CAP-34, CAP-35, CAP-36</t>
+  </si>
+  <si>
+    <t>CAP-33, CAP-34, CAP-35, CAP-36</t>
+  </si>
+  <si>
+    <t>CAP-38</t>
+  </si>
+  <si>
+    <t>CAP-44</t>
+  </si>
+  <si>
+    <t>CAP-38, CAP-44</t>
+  </si>
+  <si>
+    <t>CAP-25</t>
+  </si>
+  <si>
+    <t>CAP-26</t>
+  </si>
+  <si>
+    <t>CAP-27</t>
+  </si>
+  <si>
+    <t>CAP-28</t>
+  </si>
+  <si>
+    <t>CAP-59</t>
+  </si>
+  <si>
+    <t>CAP-25, CAP-26, CAP-27, CAP-28, CAP-59</t>
+  </si>
+  <si>
+    <t>CAP-41</t>
+  </si>
+  <si>
+    <t>CAP-45</t>
+  </si>
+  <si>
+    <t>CAP-41, CAP-45</t>
+  </si>
+  <si>
+    <t>CAP-21</t>
+  </si>
+  <si>
+    <t>CAP-22</t>
+  </si>
+  <si>
+    <t>CAP-23</t>
+  </si>
+  <si>
+    <t>CAP-24</t>
+  </si>
+  <si>
+    <t>CAP-21, CAP-22, CAP-23, CAP-24</t>
+  </si>
+  <si>
+    <t>CAP-01, CAP-03, CAP-05, CAP-07, CAP-32, CAP-14, CAP-15, CAP-16</t>
+  </si>
+  <si>
+    <t>CAP-08, CAP-13</t>
   </si>
 </sst>
 </file>
@@ -1006,7 +1186,10 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="3" builtinId="15"/>
   </cellStyles>
-  <dxfs count="79">
+  <dxfs count="81">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1244,6 +1427,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1515,10 +1701,10 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="HR_Capabilites" displayName="HR_Capabilites" ref="A2:D6" totalsRowShown="0" headerRowDxfId="62" headerRowBorderDxfId="61" tableBorderDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="HR_Capabilites" displayName="HR_Capabilites" ref="A2:D6" totalsRowShown="0" headerRowDxfId="64" headerRowBorderDxfId="63" tableBorderDxfId="62">
   <autoFilter ref="A2:D6" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Name" dataDxfId="59"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Name" dataDxfId="61"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="DIFF"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="Evidence"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="CapabilityID"/>
@@ -1531,8 +1717,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="HR_Threats" displayName="HR_Threats" ref="A9:G13" totalsRowShown="0">
   <autoFilter ref="A9:G13" xr:uid="{00000000-0009-0000-0100-000014000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="Scenario" dataDxfId="58"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0A00-000007000000}" name="TComm" dataDxfId="57"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="Scenario" dataDxfId="60"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0A00-000007000000}" name="TComm" dataDxfId="59"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="TEF"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="TC"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="LM"/>
@@ -1544,10 +1730,10 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Risk_Capabilities" displayName="Risk_Capabilities" ref="A2:D6" totalsRowShown="0" headerRowDxfId="56" headerRowBorderDxfId="55" tableBorderDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Risk_Capabilities" displayName="Risk_Capabilities" ref="A2:D6" totalsRowShown="0" headerRowDxfId="58" headerRowBorderDxfId="57" tableBorderDxfId="56">
   <autoFilter ref="A2:D6" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="Name" dataDxfId="53"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="Name" dataDxfId="55"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="DIFF"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0B00-000005000000}" name="Evidence"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" name="CapabilityID"/>
@@ -1560,8 +1746,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Risk_Threats" displayName="Risk_Threats" ref="A9:G13" totalsRowShown="0">
   <autoFilter ref="A9:G13" xr:uid="{00000000-0009-0000-0100-000017000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="Scenario" dataDxfId="52"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0C00-000007000000}" name="TComm" dataDxfId="51"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="Scenario" dataDxfId="54"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0C00-000007000000}" name="TComm" dataDxfId="53"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="TEF"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="TC"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="LM"/>
@@ -1576,8 +1762,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Policy_Threats" displayName="Policy_Threats" ref="A9:G12" totalsRowShown="0">
   <autoFilter ref="A9:G12" xr:uid="{00000000-0009-0000-0100-000019000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="Scenario" dataDxfId="50"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0D00-000007000000}" name="TComm" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="Scenario" dataDxfId="52"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0D00-000007000000}" name="TComm" dataDxfId="51"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="TEF"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0D00-000003000000}" name="TC"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0D00-000004000000}" name="LM"/>
@@ -1589,10 +1775,10 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="Policy_Capabilities" displayName="Policy_Capabilities" ref="A2:D6" totalsRowShown="0" headerRowDxfId="48" headerRowBorderDxfId="47" tableBorderDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="Policy_Capabilities" displayName="Policy_Capabilities" ref="A2:D6" totalsRowShown="0" headerRowDxfId="50" headerRowBorderDxfId="49" tableBorderDxfId="48">
   <autoFilter ref="A2:D6" xr:uid="{00000000-0009-0000-0100-00000F000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="Name" dataDxfId="45"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="Name" dataDxfId="47"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="DIFF"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0E00-000005000000}" name="Evidence"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="CapabilityID"/>
@@ -1605,7 +1791,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="ORG_Capabilities" displayName="ORG_Capabilities" ref="A2:D10" totalsRowShown="0">
   <autoFilter ref="A2:D10" xr:uid="{00000000-0009-0000-0100-000011000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="Name" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="Name" dataDxfId="46"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0F00-000004000000}" name="DIFF"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0F00-000005000000}" name="Evidence"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="CapabilityID"/>
@@ -1618,13 +1804,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="ORG_Threats" displayName="ORG_Threats" ref="A13:G18" totalsRowShown="0">
   <autoFilter ref="A13:G18" xr:uid="{00000000-0009-0000-0100-000012000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="Scenario" dataDxfId="43"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-1000-00000B000000}" name="TComm" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="Scenario" dataDxfId="45"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-1000-00000B000000}" name="TComm" dataDxfId="44"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-1000-000002000000}" name="TEF"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1000-000003000000}" name="TC"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-1000-000004000000}" name="LM"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-1000-00000D000000}" name="ScenarioID"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1000-000005000000}" name="Capabilities"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1000-000005000000}" name="Capabilities" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1634,9 +1820,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="COMP_Capabilities" displayName="COMP_Capabilities" ref="A2:D4" totalsRowShown="0">
   <autoFilter ref="A2:D4" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="Name" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="Name" dataDxfId="42"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" name="DIFF"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1100-000005000000}" name="Evidence" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1100-000005000000}" name="Evidence" dataDxfId="41"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1100-000003000000}" name="CapabilityID"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1647,8 +1833,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{00000000-000C-0000-FFFF-FFFF12000000}" name="COMP_Threats" displayName="COMP_Threats" ref="A7:G11" totalsRowShown="0">
   <autoFilter ref="A7:G11" xr:uid="{00000000-0009-0000-0100-000018000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1200-000001000000}" name="Scenario" dataDxfId="39"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1200-000007000000}" name="TComm" dataDxfId="38"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1200-000001000000}" name="Scenario" dataDxfId="40"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1200-000007000000}" name="TComm" dataDxfId="39"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-1200-000002000000}" name="TEF"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1200-000003000000}" name="TC"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-1200-000004000000}" name="LM"/>
@@ -1660,7 +1846,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table7" displayName="Table7" ref="A4:B8" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table7" displayName="Table7" ref="A4:B8" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="80">
   <sortState ref="A4:B8">
     <sortCondition descending="1" ref="A4:A8"/>
   </sortState>
@@ -1673,10 +1859,10 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF13000000}" name="Asset_Capabilities" displayName="Asset_Capabilities" ref="A2:D4" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF13000000}" name="Asset_Capabilities" displayName="Asset_Capabilities" ref="A2:D4" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37" tableBorderDxfId="36">
   <autoFilter ref="A2:D4" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1300-000001000000}" name="Name" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1300-000001000000}" name="Name" dataDxfId="35"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-1300-000002000000}" name="DIFF"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-1300-000005000000}" name="Evidence"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1300-000003000000}" name="CapabilityID"/>
@@ -1686,11 +1872,11 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{00000000-000C-0000-FFFF-FFFF14000000}" name="Asset_Threats" displayName="Asset_Threats" ref="A7:G10" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{00000000-000C-0000-FFFF-FFFF14000000}" name="Asset_Threats" displayName="Asset_Threats" ref="A7:G10" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32">
   <autoFilter ref="A7:G10" xr:uid="{00000000-0009-0000-0100-00001A000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1400-000001000000}" name="Scenario" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1400-000007000000}" name="TComm" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1400-000001000000}" name="Scenario" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1400-000007000000}" name="TComm" dataDxfId="30"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-1400-000002000000}" name="TEF"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1400-000003000000}" name="TC"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-1400-000004000000}" name="LM"/>
@@ -1705,7 +1891,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF15000000}" name="Physical_Capabilities" displayName="Physical_Capabilities" ref="A2:D6" totalsRowShown="0">
   <autoFilter ref="A2:D6" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1500-000001000000}" name="Name" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1500-000001000000}" name="Name" dataDxfId="29"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-1500-000002000000}" name="DIFF"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-1500-000005000000}" name="Evidence"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1500-000003000000}" name="CapabilityID"/>
@@ -1718,8 +1904,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF16000000}" name="Physical_Threats" displayName="Physical_Threats" ref="A9:G13" totalsRowShown="0">
   <autoFilter ref="A9:G13" xr:uid="{00000000-0009-0000-0100-000010000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1600-000001000000}" name="Scenario" dataDxfId="27"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1600-000007000000}" name="TComm" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1600-000001000000}" name="Scenario" dataDxfId="28"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1600-000007000000}" name="TComm" dataDxfId="27"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-1600-000002000000}" name="TEF"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1600-000003000000}" name="TC"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-1600-000004000000}" name="LM"/>
@@ -1734,7 +1920,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="30" xr:uid="{00000000-000C-0000-FFFF-FFFF17000000}" name="OPS_Capabilities" displayName="OPS_Capabilities" ref="A2:D16" totalsRowShown="0">
   <autoFilter ref="A2:D16" xr:uid="{00000000-0009-0000-0100-00001E000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1700-000001000000}" name="Name" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1700-000001000000}" name="Name" dataDxfId="26"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-1700-000002000000}" name="DIFF"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-1700-000005000000}" name="Evidence"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1700-000003000000}" name="CapabilityID"/>
@@ -1747,13 +1933,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{00000000-000C-0000-FFFF-FFFF18000000}" name="OPS_Threats" displayName="OPS_Threats" ref="A19:G27" totalsRowShown="0">
   <autoFilter ref="A19:G27" xr:uid="{00000000-0009-0000-0100-00001F000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1800-000001000000}" name="Scenario" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1800-000007000000}" name="TComm" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1800-000001000000}" name="Scenario" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1800-000007000000}" name="TComm" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-1800-000002000000}" name="TEF"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1800-000003000000}" name="TC"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-1800-000004000000}" name="LM"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-1800-000006000000}" name="ScenarioID"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1800-000005000000}" name="Capabilities" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1800-000005000000}" name="Capabilities" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1763,7 +1949,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{00000000-000C-0000-FFFF-FFFF19000000}" name="ADM_Capabilities" displayName="ADM_Capabilities" ref="A2:D4" totalsRowShown="0">
   <autoFilter ref="A2:D4" xr:uid="{00000000-0009-0000-0100-000013000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1900-000001000000}" name="Name" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1900-000001000000}" name="Name" dataDxfId="22"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-1900-000002000000}" name="DIFF"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-1900-000005000000}" name="Evidence"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1900-000003000000}" name="CapabilityID"/>
@@ -1776,8 +1962,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{00000000-000C-0000-FFFF-FFFF1A000000}" name="ADM_Threats" displayName="ADM_Threats" ref="A7:G8" totalsRowShown="0">
   <autoFilter ref="A7:G8" xr:uid="{00000000-0009-0000-0100-000015000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1A00-000001000000}" name="Scenario" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1A00-000007000000}" name="TComm" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1A00-000001000000}" name="Scenario" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1A00-000007000000}" name="TComm" dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-1A00-000002000000}" name="TEF"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1A00-000003000000}" name="TC"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-1A00-000004000000}" name="LM"/>
@@ -1789,10 +1975,10 @@
 </file>
 
 <file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{00000000-000C-0000-FFFF-FFFF1B000000}" name="IM_Capabilities" displayName="IM_Capabilities" ref="A2:D7" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{00000000-000C-0000-FFFF-FFFF1B000000}" name="IM_Capabilities" displayName="IM_Capabilities" ref="A2:D7" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17">
   <autoFilter ref="A2:D7" xr:uid="{00000000-0009-0000-0100-000020000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1B00-000001000000}" name="Name" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1B00-000001000000}" name="Name" dataDxfId="16"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-1B00-000002000000}" name="DIFF"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-1B00-000005000000}" name="Evidence"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1B00-000003000000}" name="CapabilityID"/>
@@ -1802,23 +1988,23 @@
 </file>
 
 <file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{00000000-000C-0000-FFFF-FFFF1C000000}" name="IM_Threats" displayName="IM_Threats" ref="A10:G22" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{00000000-000C-0000-FFFF-FFFF1C000000}" name="IM_Threats" displayName="IM_Threats" ref="A10:G22" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13">
   <autoFilter ref="A10:G22" xr:uid="{00000000-0009-0000-0100-000021000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1C00-000001000000}" name="Scenario" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1C00-000007000000}" name="TComm" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1C00-000001000000}" name="Scenario" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1C00-000007000000}" name="TComm" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-1C00-000002000000}" name="TEF"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1C00-000003000000}" name="TC"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-1C00-000004000000}" name="LM"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-1C00-000006000000}" name="ScenarioID"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1C00-000005000000}" name="Capabilities" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1C00-000005000000}" name="Capabilities" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table8" displayName="Table8" ref="A11:B13" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="77">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table8" displayName="Table8" ref="A11:B13" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="79">
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Column2" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4"/>
@@ -1831,7 +2017,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="28" xr:uid="{00000000-000C-0000-FFFF-FFFF1D000000}" name="BC_Capabilities" displayName="BC_Capabilities" ref="A2:D4" totalsRowShown="0">
   <autoFilter ref="A2:D4" xr:uid="{00000000-0009-0000-0100-00001C000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1D00-000001000000}" name="Name" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1D00-000001000000}" name="Name" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-1D00-000002000000}" name="DIFF"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-1D00-000005000000}" name="Evidence"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1D00-000003000000}" name="CapabilityID"/>
@@ -1844,8 +2030,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{00000000-000C-0000-FFFF-FFFF1E000000}" name="BC_Threats" displayName="BC_Threats" ref="A7:G9" totalsRowShown="0">
   <autoFilter ref="A7:G9" xr:uid="{00000000-0009-0000-0100-00001D000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1E00-000001000000}" name="Scenario" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1E00-000007000000}" name="TComm" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1E00-000001000000}" name="Scenario" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1E00-000007000000}" name="TComm" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-1E00-000002000000}" name="TEF"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1E00-000003000000}" name="TC"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-1E00-000004000000}" name="LM"/>
@@ -1857,10 +2043,10 @@
 </file>
 
 <file path=xl/tables/table32.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF1F000000}" name="Privacy_Capabilities" displayName="Privacy_Capabilities" ref="A2:D6" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF1F000000}" name="Privacy_Capabilities" displayName="Privacy_Capabilities" ref="A2:D6" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
   <autoFilter ref="A2:D6" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1F00-000001000000}" name="Name" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1F00-000001000000}" name="Name" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-1F00-000002000000}" name="DIFF"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-1F00-000005000000}" name="Evidence"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1F00-000003000000}" name="CapabilityID"/>
@@ -1873,20 +2059,20 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{00000000-000C-0000-FFFF-FFFF20000000}" name="Privacy_Threats" displayName="Privacy_Threats" ref="A9:G12" totalsRowShown="0">
   <autoFilter ref="A9:G12" xr:uid="{00000000-0009-0000-0100-000016000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2000-000001000000}" name="Scenario" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-2000-000007000000}" name="TComm" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2000-000001000000}" name="Scenario" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-2000-000007000000}" name="TComm" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-2000-000002000000}" name="TEF"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-2000-000003000000}" name="TC"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-2000-000004000000}" name="LM"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-2000-000006000000}" name="ScenarioID"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2000-000005000000}" name="Capabilities"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2000-000005000000}" name="Capabilities" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table9" displayName="Table9" ref="A16:B18" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table9" displayName="Table9" ref="A16:B18" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="78">
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Column2" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4"/>
@@ -1896,7 +2082,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table11" displayName="Table11" ref="A21:B23" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table11" displayName="Table11" ref="A21:B23" headerRowCount="0" totalsRowShown="0" tableBorderDxfId="77">
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Column2" headerRowCellStyle="20% - Accent4" dataCellStyle="20% - Accent4"/>
@@ -1909,7 +2095,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="ISMP_Capabilities" displayName="ISMP_Capabilities" ref="A2:D5" totalsRowShown="0">
   <autoFilter ref="A2:D5" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Name" dataDxfId="74"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Name" dataDxfId="76"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="DIFF"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Evidence"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="CapabilityID"/>
@@ -1922,8 +2108,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="ISMP_Threats" displayName="ISMP_Threats" ref="A8:G9" totalsRowShown="0">
   <autoFilter ref="A8:G9" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Scenario" dataDxfId="73"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="TComm" dataDxfId="72"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Scenario" dataDxfId="75"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="TComm" dataDxfId="74"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="TEF"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="TC"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="LM"/>
@@ -1935,10 +2121,10 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="AC_Capabilities" displayName="AC_Capabilities" ref="A2:D4" totalsRowShown="0" headerRowDxfId="71" headerRowBorderDxfId="70" tableBorderDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="AC_Capabilities" displayName="AC_Capabilities" ref="A2:D4" totalsRowShown="0" headerRowDxfId="73" headerRowBorderDxfId="72" tableBorderDxfId="71">
   <autoFilter ref="A2:D4" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Name" dataDxfId="68"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Name" dataDxfId="70"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="DIFF"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Evidence"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="CapabilityID"/>
@@ -1948,11 +2134,11 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="AC_Threats" displayName="AC_Threats" ref="A7:G9" totalsRowShown="0" headerRowDxfId="67" headerRowBorderDxfId="66" tableBorderDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="AC_Threats" displayName="AC_Threats" ref="A7:G9" totalsRowShown="0" headerRowDxfId="69" headerRowBorderDxfId="68" tableBorderDxfId="67">
   <autoFilter ref="A7:G9" xr:uid="{00000000-0009-0000-0100-00001B000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Scenario" dataDxfId="64"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="TComm" dataDxfId="63"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Scenario" dataDxfId="66"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="TComm" dataDxfId="65"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="TEF"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="TC"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="LM"/>
@@ -2274,144 +2460,144 @@
   <sheetData>
     <row r="1" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -2448,8 +2634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2458,8 +2644,7 @@
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20" x14ac:dyDescent="0.25">
@@ -2486,30 +2671,30 @@
     </row>
     <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B3" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C3" t="s">
         <v>43</v>
       </c>
-      <c r="D3">
-        <v>8</v>
+      <c r="D3" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B4" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D4">
-        <v>13</v>
+      <c r="D4" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="20" x14ac:dyDescent="0.25">
@@ -2548,10 +2733,10 @@
     </row>
     <row r="8" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -2563,10 +2748,10 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
       <c r="G8" t="s">
-        <v>146</v>
+        <v>334</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -2586,10 +2771,10 @@
         <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="G9" t="s">
-        <v>146</v>
+        <v>334</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -2597,7 +2782,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -2609,10 +2794,10 @@
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="G10" t="s">
-        <v>146</v>
+        <v>334</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -2620,7 +2805,7 @@
         <v>17</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -2632,10 +2817,10 @@
         <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
       <c r="G11" t="s">
-        <v>146</v>
+        <v>334</v>
       </c>
     </row>
   </sheetData>
@@ -2671,7 +2856,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2708,30 +2893,30 @@
     </row>
     <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="C3" t="s">
         <v>43</v>
       </c>
-      <c r="D3">
-        <v>56</v>
+      <c r="D3" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B4" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="C4" t="s">
         <v>43</v>
       </c>
-      <c r="D4">
-        <v>39</v>
+      <c r="D4" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -2788,15 +2973,15 @@
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="G8" t="s">
-        <v>147</v>
+        <v>294</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>42</v>
@@ -2811,15 +2996,15 @@
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="G9" t="s">
-        <v>147</v>
+        <v>294</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>42</v>
@@ -2834,10 +3019,10 @@
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="G10" t="s">
-        <v>147</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -2873,7 +3058,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2883,7 +3068,7 @@
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20" x14ac:dyDescent="0.2">
@@ -2910,58 +3095,58 @@
     </row>
     <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="C3" t="s">
         <v>43</v>
       </c>
-      <c r="D3">
-        <v>52</v>
+      <c r="D3" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="C4" t="s">
         <v>43</v>
       </c>
-      <c r="D4">
-        <v>53</v>
+      <c r="D4" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B5" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="C5" t="s">
         <v>43</v>
       </c>
-      <c r="D5">
-        <v>54</v>
+      <c r="D5" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="C6" t="s">
         <v>43</v>
       </c>
-      <c r="D6">
-        <v>55</v>
+      <c r="D6" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="20" x14ac:dyDescent="0.2">
@@ -3000,10 +3185,10 @@
     </row>
     <row r="10" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -3015,10 +3200,10 @@
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="G10" t="s">
-        <v>148</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -3026,7 +3211,7 @@
         <v>37</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -3038,10 +3223,10 @@
         <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="G11" t="s">
-        <v>148</v>
+        <v>299</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -3061,10 +3246,10 @@
         <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="G12" t="s">
-        <v>148</v>
+        <v>299</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -3072,7 +3257,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -3084,10 +3269,10 @@
         <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="G13" t="s">
-        <v>148</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -3095,7 +3280,7 @@
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A8:G8"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="4">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10:C13" xr:uid="{00000000-0002-0000-0B00-000000000000}">
       <formula1>TEF_Values</formula1>
     </dataValidation>
@@ -3122,8 +3307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3160,198 +3345,198 @@
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B3" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="C3" t="s">
         <v>43</v>
       </c>
-      <c r="D3">
-        <v>37</v>
+      <c r="D3" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B4" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="C4" t="s">
         <v>43</v>
       </c>
-      <c r="D4">
-        <v>40</v>
+      <c r="D4" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B5" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C5" t="s">
         <v>43</v>
       </c>
-      <c r="D5">
-        <v>42</v>
+      <c r="D5" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B6" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="C6" t="s">
         <v>43</v>
       </c>
-      <c r="D6">
-        <v>43</v>
+      <c r="D6" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B7" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C7" t="s">
         <v>43</v>
       </c>
-      <c r="D7">
-        <v>46</v>
+      <c r="D7" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B8" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C8" t="s">
         <v>43</v>
       </c>
-      <c r="D8">
-        <v>47</v>
+      <c r="D8" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B9" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C9" t="s">
         <v>43</v>
       </c>
-      <c r="D9">
-        <v>48</v>
+      <c r="D9" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B10" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="C10" t="s">
         <v>43</v>
       </c>
-      <c r="D10">
-        <v>49</v>
+      <c r="D10" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B11" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="C11" t="s">
         <v>43</v>
       </c>
-      <c r="D11">
-        <v>50</v>
+      <c r="D11" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B12" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="C12" t="s">
         <v>43</v>
       </c>
-      <c r="D12">
-        <v>51</v>
+      <c r="D12" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="B13" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="C13" t="s">
         <v>43</v>
       </c>
-      <c r="D13">
-        <v>33</v>
+      <c r="D13" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B14" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="C14" t="s">
         <v>43</v>
       </c>
-      <c r="D14">
-        <v>34</v>
+      <c r="D14" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B15" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="C15" t="s">
         <v>43</v>
       </c>
-      <c r="D15">
-        <v>35</v>
+      <c r="D15" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B16" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="C16" t="s">
         <v>43</v>
       </c>
-      <c r="D16">
-        <v>36</v>
+      <c r="D16" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -3391,9 +3576,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="B20" t="s">
         <v>42</v>
@@ -3408,13 +3593,13 @@
         <v>9</v>
       </c>
       <c r="F20" t="s">
-        <v>249</v>
+        <v>231</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>32</v>
       </c>
@@ -3431,18 +3616,18 @@
         <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
@@ -3454,18 +3639,18 @@
         <v>9</v>
       </c>
       <c r="F22" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
@@ -3477,18 +3662,18 @@
         <v>10</v>
       </c>
       <c r="F23" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
@@ -3500,18 +3685,18 @@
         <v>10</v>
       </c>
       <c r="F24" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>151</v>
+        <v>314</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="B25" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="C25" t="s">
         <v>7</v>
@@ -3523,18 +3708,18 @@
         <v>10</v>
       </c>
       <c r="F25" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>200</v>
+        <v>315</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="B26" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="C26" t="s">
         <v>12</v>
@@ -3546,18 +3731,18 @@
         <v>10</v>
       </c>
       <c r="F26" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>200</v>
+        <v>315</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="C27" t="s">
         <v>12</v>
@@ -3569,10 +3754,10 @@
         <v>9</v>
       </c>
       <c r="F27" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>200</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -3607,7 +3792,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3643,30 +3828,30 @@
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="C3" t="s">
         <v>43</v>
       </c>
-      <c r="D3">
-        <v>38</v>
+      <c r="D3" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="C4" t="s">
         <v>43</v>
       </c>
-      <c r="D4">
-        <v>44</v>
+      <c r="D4" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="20" x14ac:dyDescent="0.2">
@@ -3720,10 +3905,10 @@
         <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="G8" t="s">
-        <v>161</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -3758,8 +3943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3796,72 +3981,72 @@
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="C3" t="s">
         <v>43</v>
       </c>
-      <c r="D3">
-        <v>25</v>
+      <c r="D3" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="B4" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="C4" t="s">
         <v>43</v>
       </c>
-      <c r="D4">
-        <v>26</v>
+      <c r="D4" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B5" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C5" t="s">
         <v>43</v>
       </c>
-      <c r="D5">
-        <v>27</v>
+      <c r="D5" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B6" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C6" t="s">
         <v>43</v>
       </c>
-      <c r="D6">
-        <v>28</v>
+      <c r="D6" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B7" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="C7" t="s">
         <v>43</v>
       </c>
-      <c r="D7">
-        <v>59</v>
+      <c r="D7" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="20" x14ac:dyDescent="0.25">
@@ -3898,7 +4083,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>41</v>
       </c>
@@ -3915,15 +4100,15 @@
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>203</v>
+        <v>185</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>42</v>
@@ -3938,13 +4123,13 @@
         <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>25</v>
       </c>
@@ -3961,18 +4146,18 @@
         <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
@@ -3984,18 +4169,18 @@
         <v>9</v>
       </c>
       <c r="F14" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
@@ -4007,18 +4192,18 @@
         <v>9</v>
       </c>
       <c r="F15" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
@@ -4030,10 +4215,10 @@
         <v>9</v>
       </c>
       <c r="F16" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>149</v>
+        <v>324</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -4041,7 +4226,7 @@
         <v>28</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -4053,10 +4238,10 @@
         <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>264</v>
-      </c>
-      <c r="G17" s="3">
-        <v>59</v>
+        <v>246</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -4076,18 +4261,18 @@
         <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>265</v>
-      </c>
-      <c r="G18" s="3">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>247</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
@@ -4099,18 +4284,18 @@
         <v>9</v>
       </c>
       <c r="F19" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
@@ -4122,18 +4307,18 @@
         <v>9</v>
       </c>
       <c r="F20" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
@@ -4145,15 +4330,15 @@
         <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>42</v>
@@ -4168,10 +4353,10 @@
         <v>9</v>
       </c>
       <c r="F22" t="s">
-        <v>269</v>
+        <v>251</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>149</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -4179,7 +4364,7 @@
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A9:G9"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="4">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B7" xr:uid="{00000000-0002-0000-0E00-000000000000}">
       <formula1>DIFF_Values</formula1>
     </dataValidation>
@@ -4207,7 +4392,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4243,30 +4428,30 @@
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="C3" t="s">
         <v>43</v>
       </c>
-      <c r="D3">
-        <v>41</v>
+      <c r="D3" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="C4" t="s">
         <v>43</v>
       </c>
-      <c r="D4">
-        <v>45</v>
+      <c r="D4" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="20" x14ac:dyDescent="0.2">
@@ -4305,10 +4490,10 @@
     </row>
     <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -4320,10 +4505,10 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="G8" t="s">
-        <v>150</v>
+        <v>327</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -4343,10 +4528,10 @@
         <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
       <c r="G9" t="s">
-        <v>150</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -4381,8 +4566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4419,58 +4604,58 @@
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C3" t="s">
         <v>43</v>
       </c>
-      <c r="D3">
-        <v>21</v>
+      <c r="D3" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="C4" t="s">
         <v>43</v>
       </c>
-      <c r="D4">
-        <v>22</v>
+      <c r="D4" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B5" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="C5" t="s">
         <v>43</v>
       </c>
-      <c r="D5">
-        <v>23</v>
+      <c r="D5" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B6" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="C6" t="s">
         <v>43</v>
       </c>
-      <c r="D6">
-        <v>24</v>
+      <c r="D6" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="20" x14ac:dyDescent="0.25">
@@ -4524,10 +4709,10 @@
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>272</v>
-      </c>
-      <c r="G10" t="s">
-        <v>48</v>
+        <v>254</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -4535,7 +4720,7 @@
         <v>23</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -4547,10 +4732,10 @@
         <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>273</v>
-      </c>
-      <c r="G11" t="s">
-        <v>48</v>
+        <v>255</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -4570,10 +4755,10 @@
         <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>274</v>
-      </c>
-      <c r="G12" t="s">
-        <v>48</v>
+        <v>256</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -4620,59 +4805,59 @@
   <sheetData>
     <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="B1" s="10"/>
     </row>
     <row r="3" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="B3" s="11"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="B10" s="11"/>
     </row>
@@ -4681,7 +4866,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -4689,7 +4874,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -4697,12 +4882,12 @@
         <v>10</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="B15" s="11"/>
     </row>
@@ -4711,7 +4896,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -4719,7 +4904,7 @@
         <v>12</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -4727,12 +4912,12 @@
         <v>8</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="20" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="B20" s="11"/>
     </row>
@@ -4741,7 +4926,7 @@
         <v>11</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -4749,7 +4934,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -4757,7 +4942,7 @@
         <v>10</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -4859,27 +5044,27 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -4892,7 +5077,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4929,44 +5114,44 @@
     </row>
     <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C3" t="s">
         <v>43</v>
       </c>
-      <c r="D3">
-        <v>2</v>
+      <c r="D3" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C4" t="s">
         <v>43</v>
       </c>
-      <c r="D4">
-        <v>4</v>
+      <c r="D4" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="C5" t="s">
         <v>43</v>
       </c>
-      <c r="D5">
-        <v>6</v>
+      <c r="D5" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="20" x14ac:dyDescent="0.2">
@@ -5005,10 +5190,10 @@
     </row>
     <row r="9" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -5020,10 +5205,10 @@
         <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="G9" t="s">
-        <v>144</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -5059,7 +5244,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5096,30 +5281,30 @@
     </row>
     <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C3" t="s">
         <v>43</v>
       </c>
-      <c r="D3">
-        <v>57</v>
+      <c r="D3" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="C4" t="s">
         <v>43</v>
       </c>
-      <c r="D4">
-        <v>58</v>
+      <c r="D4" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="20" x14ac:dyDescent="0.25">
@@ -5173,18 +5358,18 @@
         <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="G8" t="s">
-        <v>49</v>
+        <v>263</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -5196,10 +5381,10 @@
         <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="G9" t="s">
-        <v>49</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -5235,7 +5420,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5245,7 +5430,7 @@
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20" x14ac:dyDescent="0.25">
@@ -5272,58 +5457,58 @@
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C3" t="s">
         <v>43</v>
       </c>
-      <c r="D3">
-        <v>29</v>
+      <c r="D3" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="C4" t="s">
         <v>43</v>
       </c>
-      <c r="D4">
-        <v>30</v>
+      <c r="D4" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="C5" t="s">
         <v>43</v>
       </c>
-      <c r="D5">
-        <v>31</v>
+      <c r="D5" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B6" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C6" t="s">
         <v>43</v>
       </c>
-      <c r="D6">
-        <v>60</v>
+      <c r="D6" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="20" x14ac:dyDescent="0.25">
@@ -5362,7 +5547,7 @@
     </row>
     <row r="10" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>42</v>
@@ -5377,10 +5562,10 @@
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="G10" t="s">
-        <v>192</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -5400,15 +5585,15 @@
         <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="G11" t="s">
-        <v>145</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>42</v>
@@ -5423,18 +5608,18 @@
         <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="G12" t="s">
-        <v>192</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -5446,10 +5631,10 @@
         <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="G13" t="s">
-        <v>145</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -5485,7 +5670,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5496,7 +5681,7 @@
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20" x14ac:dyDescent="0.25">
@@ -5523,58 +5708,58 @@
     </row>
     <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C3" t="s">
         <v>43</v>
       </c>
-      <c r="D3">
-        <v>17</v>
+      <c r="D3" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="C4" t="s">
         <v>43</v>
       </c>
-      <c r="D4">
-        <v>18</v>
+      <c r="D4" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="C5" t="s">
         <v>43</v>
       </c>
-      <c r="D5">
-        <v>19</v>
+      <c r="D5" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="C6" t="s">
         <v>43</v>
       </c>
-      <c r="D6">
-        <v>20</v>
+      <c r="D6" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="20" x14ac:dyDescent="0.25">
@@ -5613,10 +5798,10 @@
     </row>
     <row r="10" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
@@ -5628,10 +5813,10 @@
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="G10" t="s">
-        <v>47</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -5639,7 +5824,7 @@
         <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -5651,10 +5836,10 @@
         <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
       <c r="G11" t="s">
-        <v>47</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -5662,7 +5847,7 @@
         <v>20</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -5674,15 +5859,15 @@
         <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="G12" t="s">
-        <v>47</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>42</v>
@@ -5697,10 +5882,10 @@
         <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="G13" t="s">
-        <v>47</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -5736,7 +5921,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5747,7 +5932,7 @@
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20" x14ac:dyDescent="0.25">
@@ -5774,58 +5959,58 @@
     </row>
     <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C3" t="s">
         <v>43</v>
       </c>
-      <c r="D3">
-        <v>9</v>
+      <c r="D3" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="C4" t="s">
         <v>43</v>
       </c>
-      <c r="D4">
-        <v>10</v>
+      <c r="D4" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C5" t="s">
         <v>43</v>
       </c>
-      <c r="D5">
-        <v>11</v>
+      <c r="D5" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C6" t="s">
         <v>43</v>
       </c>
-      <c r="D6">
-        <v>12</v>
+      <c r="D6" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -5867,7 +6052,7 @@
     </row>
     <row r="10" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>42</v>
@@ -5882,15 +6067,15 @@
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="G10" t="s">
-        <v>46</v>
+        <v>279</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>42</v>
@@ -5905,15 +6090,15 @@
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="G11" t="s">
-        <v>46</v>
+        <v>279</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>42</v>
@@ -5928,10 +6113,10 @@
         <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="G12" t="s">
-        <v>46</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -5966,8 +6151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5976,7 +6161,7 @@
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20" x14ac:dyDescent="0.25">
@@ -6003,114 +6188,114 @@
     </row>
     <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="C3" t="s">
         <v>43</v>
       </c>
-      <c r="D3">
-        <v>1</v>
+      <c r="D3" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C4" t="s">
         <v>43</v>
       </c>
-      <c r="D4">
-        <v>3</v>
+      <c r="D4" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C5" t="s">
         <v>43</v>
       </c>
-      <c r="D5">
-        <v>5</v>
+      <c r="D5" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="C6" t="s">
         <v>43</v>
       </c>
-      <c r="D6">
-        <v>7</v>
+      <c r="D6" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B7" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C7" t="s">
         <v>43</v>
       </c>
-      <c r="D7">
-        <v>32</v>
+      <c r="D7" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B8" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D8">
-        <v>14</v>
+      <c r="D8" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B9" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D9">
-        <v>15</v>
+      <c r="D9" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B10" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D10">
-        <v>16</v>
+      <c r="D10" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="20" x14ac:dyDescent="0.2">
@@ -6149,10 +6334,10 @@
     </row>
     <row r="14" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
@@ -6164,18 +6349,18 @@
         <v>9</v>
       </c>
       <c r="F14" t="s">
-        <v>233</v>
-      </c>
-      <c r="G14" t="s">
-        <v>197</v>
+        <v>215</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
@@ -6187,18 +6372,18 @@
         <v>9</v>
       </c>
       <c r="F15" t="s">
-        <v>234</v>
-      </c>
-      <c r="G15" t="s">
-        <v>197</v>
+        <v>216</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
@@ -6210,10 +6395,10 @@
         <v>9</v>
       </c>
       <c r="F16" t="s">
-        <v>235</v>
-      </c>
-      <c r="G16" t="s">
-        <v>197</v>
+        <v>217</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -6221,7 +6406,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
@@ -6233,18 +6418,18 @@
         <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>236</v>
-      </c>
-      <c r="G17" t="s">
-        <v>196</v>
+        <v>218</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
@@ -6256,10 +6441,10 @@
         <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>237</v>
-      </c>
-      <c r="G18" t="s">
-        <v>195</v>
+        <v>219</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>